<commit_message>
Updated tooltips for babies
</commit_message>
<xml_diff>
--- a/game/dota_addons/vampirism/resource/VampToolTipHelp.xlsx
+++ b/game/dota_addons/vampirism/resource/VampToolTipHelp.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="1299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="1373">
   <si>
     <t>Seal</t>
   </si>
@@ -3923,6 +3923,228 @@
   </si>
   <si>
     <t>Meta Info</t>
+  </si>
+  <si>
+    <t>Summons an electrical charge to hit a slayer then bounce to another nearby dealing 5000 damage to both.|n|n|cff93C4F4Cooldown: 30 seconds.</t>
+  </si>
+  <si>
+    <t>A ring Infused with the power of bats.|n|cff93C4F4Deals 50 damage every .2 seconds|n|n|cffff0000Having more than two has no effect</t>
+  </si>
+  <si>
+    <t>Gives 1 gold to the player on pickup.</t>
+  </si>
+  <si>
+    <t>Increases your damage by 4000 and stats by 750.</t>
+  </si>
+  <si>
+    <t>Heals &lt;AIha,DataA1&gt; hit points to all friendly non-mechanical units around the Hero when used.</t>
+  </si>
+  <si>
+    <t>Gives 2 gold to the player on pickup.</t>
+  </si>
+  <si>
+    <t>Lets you farsight every 30 seconds and gives you some gold every minute. The amount of gold increases with game time.|n|nLimited to one per person (does not stack).|n|n|cffc0c0c0Available at 11 minute mark|r</t>
+  </si>
+  <si>
+    <t>Increases all stats by 2000 and attack by 500</t>
+  </si>
+  <si>
+    <t>The Second Of The Unholy Gauntlet Set, gives +500 to all stats and each subsequent attack on the same target deals 50 more damage.</t>
+  </si>
+  <si>
+    <t>Summons a Rod that produces blight</t>
+  </si>
+  <si>
+    <t>Summons a huge grave that damages nearby units. Range is 1200. |n|n|cff93C4F4Build Time: 20 seconds</t>
+  </si>
+  <si>
+    <t>Teleports the Hero to the targeted allied land unit or structure.</t>
+  </si>
+  <si>
+    <t>Adds &lt;AIpb,DataA1&gt; bonus damage to the attack of a Hero when carried. The Hero's attacks also become ranged when attacking air and poison enemy units for &lt;Apo2,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Gives short temporary damage boost. Also gives higher hit point and mana regeneration.</t>
+  </si>
+  <si>
+    <t>Does 2000 damage to any targeted structure in a distance then ricochets to 2 others.|n|n|cff93C4F4Cooldown: 30 seconds|n|n|cffFF0000Does not stack with Burst Gem or Pulse Staff</t>
+  </si>
+  <si>
+    <t>Gives the player vision of a target hero for 30 seconds or target unit for 2 minutes.</t>
+  </si>
+  <si>
+    <t>Increases the movement speed of the Hero and nearby allied units to the maximum movement speed. |nLasts &lt;AIsa,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Gives friendly nearby units a &lt;AIrr,DataA1,%&gt;% bonus to damage for &lt;AIrr,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Teleports the Vampire to safe ground after 10 seconds. Can only be used once!</t>
+  </si>
+  <si>
+    <t>Increases the HP capacity of the Hero by 10000 when worn.</t>
+  </si>
+  <si>
+    <t>Drops a ward that heals nearby friendly units for &lt;Ahwd,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Gives you immunity to all spells except Ensnare.</t>
+  </si>
+  <si>
+    <t>Restores &lt;AIm1,DataA1&gt; mana when used.</t>
+  </si>
+  <si>
+    <t>Increases all stats by 300 (200 to agility)</t>
+  </si>
+  <si>
+    <t>A powerful jewel onced use by the hands of the legendary vampire slayer before he was killed by Dracula. Used to give a great boost in power once activated.</t>
+  </si>
+  <si>
+    <t>|cff87ceebNon-Combat Consumable|r|nRegenerates the Hero's mana by &lt;AIpl,DataB1&gt; over &lt;AIpl,Dur1&gt; seconds when used.</t>
+  </si>
+  <si>
+    <t>Increases the attack damage of the Hero by 20.</t>
+  </si>
+  <si>
+    <t>Causes an eclipse that blocks out the sun and creates an artificial night. |nLasts &lt;AIct,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Teleports a target unit to your highest level town hall, stunning the unit and regenerating &lt;ANsa,DataE1&gt; hit points per second. Lasts until the unit is fully healed.</t>
+  </si>
+  <si>
+    <t>Teleports a target friendly unit to its highest level town hall.</t>
+  </si>
+  <si>
+    <t>Increases movement speed by +60 and gives Bloodlust ability.</t>
+  </si>
+  <si>
+    <t>Turns invisible for 10 minutes. The effect is loss once this Hero attacks or casts a spell, useless if you have the Cloak of Shadows. While carrying this, your speed is increased.</t>
+  </si>
+  <si>
+    <t>Creates two Skeleton Warriors from a corpse. |nContains &lt;rnec,uses&gt; charges.</t>
+  </si>
+  <si>
+    <t>Creates an area of Blight at a target location.</t>
+  </si>
+  <si>
+    <t>Heals &lt;AIh1,DataA1&gt; hit points when used.</t>
+  </si>
+  <si>
+    <t>Increases the vampire's hit point regeneration by 20 hit points per second.</t>
+  </si>
+  <si>
+    <t>Deals 1500 damage to nearby structures.</t>
+  </si>
+  <si>
+    <t>Boosts attack by 2000 and gives a +250 bonus to all stats.|n|n|cffc0c0c0Available at 25 minute mark.|r</t>
+  </si>
+  <si>
+    <t>Allows the Hero to cast Cyclone. Cyclone tosses a target enemy unit into the air, rendering it unable to attack, move or cast spells. |nLasts &lt;AIcy,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Automatically brings the Hero back to life with &lt;AIrc,DataB1&gt; hit points when the Hero wearing the Ankh dies.</t>
+  </si>
+  <si>
+    <t>Gives the Hero immunity to magical spells for &lt;AIxs,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Adds &lt;AIfb,DataA1&gt; bonus fire damage to the attack of a Hero when carried. The Hero's attacks also become ranged when attacking air and do splash damage to nearby enemy units.</t>
+  </si>
+  <si>
+    <t>|cff87ceebNon-Combat Consumable|r|nRegenerates the hit points of all friendly non-mechanical units in an area around your Hero by &lt;AIsl,DataA1&gt; over &lt;AIsl,Dur1&gt; seconds when used.</t>
+  </si>
+  <si>
+    <t>Does 2000 damage to any targeted structure in a distance then ricochets to 2 others.|n|cff8b00ff-Requires-|n|cffF97C00Pulse Staff|nBurst Gem</t>
+  </si>
+  <si>
+    <t>|cff87ceebNon-Combat Consumable|r|nRegenerates &lt;AIp3,DataA1&gt; hit points and &lt;AIp3,DataB1&gt; mana of the Hero over &lt;AIp3,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Gives the Vampire permanent invisibility, even while attacking.</t>
+  </si>
+  <si>
+    <t>Creates a Venom Spire.</t>
+  </si>
+  <si>
+    <t>Increases your vampire's hit point regeneration by 20 hit points per second.</t>
+  </si>
+  <si>
+    <t>|cff87ceebNon-Combat Consumable|r|nRegenerates a target unit's hit points by &lt;AIrl,DataA1&gt; over &lt;AIrl,Dur1&gt; seconds when used. |nContains &lt;hslv,uses&gt; charges.</t>
+  </si>
+  <si>
+    <t>Increases the armor of the Hero by 1.</t>
+  </si>
+  <si>
+    <t>Reveals enemy invisible units in an area around the Hero. |nContains &lt;dust,uses&gt; charges. |nLasts &lt;AItb,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Adds &lt;AIcb,DataA1&gt; bonus damage to the attack of a Hero when carried. The Hero's attacks also become ranged when attacking air and reduce the armor of enemy units for &lt;AIcb,Dur1&gt; seconds.</t>
+  </si>
+  <si>
+    <t>Grants +3000 HP and +300 attack.</t>
+  </si>
+  <si>
+    <t>Makes the vampire invulnerable to damage for 15 seconds when used. An invulnerable vampire may not be the target of spells or effects. Unlimited uses. |n|nCooldown: 150 seconds</t>
+  </si>
+  <si>
+    <t>Does 1500 damage to any targeted structure in a distance.|nCooldown: 30 seconds|nDoes not stack with Ricochet Gem</t>
+  </si>
+  <si>
+    <t>Permanently increases the damage of the Hero by 100.</t>
+  </si>
+  <si>
+    <t>Powerful attire for Slayers that boosts damage by 300, HP by 3000, and gives the ability to see invisible units.</t>
+  </si>
+  <si>
+    <t>Creates a Great Hall at a target location. Human, Night Elf, and Undead players will get their racial equivalent town hall.</t>
+  </si>
+  <si>
+    <t>Drops a Sentry Ward to spy upon an area for &lt;A03A,Dur1&gt; seconds. |nContains &lt;I014,uses&gt; charges.</t>
+  </si>
+  <si>
+    <t>Restores 25000 hit points/mana and debuffs all negative buffs from the user.|n|n|cff93C4F4Cooldown: 450 seconds</t>
+  </si>
+  <si>
+    <t>Imbued with (almost) all Dracula's power. Gives 6000 damage, 2500 to all stats and permanent invisibility.</t>
+  </si>
+  <si>
+    <t>Allows the Hero to detect hidden or invisible units in the Hero's line of sight when carried.</t>
+  </si>
+  <si>
+    <t>When gazing into this crystal ball, a Slayer can see how many infernals there exists in this world.</t>
+  </si>
+  <si>
+    <t>Prevents all enemies in a targetted area from using spells for 30 seconds.|n|n|cffc0c0c0Available at 12 minute mark.|r</t>
+  </si>
+  <si>
+    <t>Summons 4 Engineers.  Engineers last 2 minutes. (Beware of the felbeasts who's main goal is to destroy your Engineers!)|n|n|cff93C4F4Cooldown: 3 minutes</t>
+  </si>
+  <si>
+    <t>A specially made teleportation staff for your Human. Teleports your human to a friendly or allied structure.|n|n|cff93C4F4Cooldown: 10 seconds</t>
+  </si>
+  <si>
+    <t>Imbued with (almost) all Dracula's power. Gives 6000 damage, 2500 to all stats and permanent invisibility.|n-Requires-|nCloak of Shadows|nDemonic Remains|nGauntlets of the Underworld</t>
+  </si>
+  <si>
+    <t>Increases the mana capacity of the Hero by 10000 when worn.</t>
+  </si>
+  <si>
+    <t>Adds &lt;AIll,DataA1&gt; bonus damage to the attack of a Hero when carried. The Hero's attacks also become ranged when attacking air, and have a chance to dispel magic and slow the movement speed of the enemy for &lt;AIlp,Dur1&gt; seconds. |n|cffffcc00Deals &lt;AIpg,DataC1&gt; bonus damage to summoned units.</t>
+  </si>
+  <si>
+    <t>Creates a player-controlled critter that can be used to scout enemies.</t>
+  </si>
+  <si>
+    <t>A legendary circlet that houses the spirit of a legendary vampire hunter. Any slayer that wears this will be able to destroy vampires with ease.</t>
+  </si>
+  <si>
+    <t>Creates a Scout Tower at a target location.</t>
+  </si>
+  <si>
+    <t>An orb that gives 5 stats every 15 seconds to all vampires, and gives the holder a VERY short blink (enough to blink across ONE wall, tree or cliff).|n|nBlink starts with two charges, which restore themselves 30 seconds after usage.|n|n|cffff0000Stats per second(s) do not stack.|nMultiple Spheres don't give more charges.|r</t>
+  </si>
+  <si>
+    <t>Pleb Tips</t>
   </si>
 </sst>
 </file>
@@ -29455,19 +29677,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="110.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1091</v>
       </c>
@@ -29475,520 +29698,574 @@
         <v>1092</v>
       </c>
       <c r="C1" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D1" t="s">
         <v>1252</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1253</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1093</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1094</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1095</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1096</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>1298</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1097</v>
       </c>
       <c r="B2" t="s">
         <v>1098</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>1097</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>1097</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1099</v>
       </c>
       <c r="B3" t="s">
         <v>1100</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>1299</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>175</v>
       </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="b">
         <v>1</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>120</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1101</v>
       </c>
       <c r="B4" t="s">
         <v>1102</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>1300</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>300</v>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="b">
         <v>1</v>
       </c>
       <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1103</v>
       </c>
       <c r="B5" t="s">
         <v>1104</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>1301</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
       </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1105</v>
       </c>
       <c r="B6" t="s">
         <v>1106</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>1302</v>
       </c>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>2000</v>
       </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="b">
         <v>1</v>
       </c>
       <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>120</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>1254</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1107</v>
       </c>
       <c r="B7" t="s">
         <v>1108</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>1303</v>
       </c>
       <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>250</v>
       </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>120</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>1255</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1109</v>
       </c>
       <c r="B8" t="s">
         <v>1110</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="C8" t="s">
+        <v>1304</v>
       </c>
       <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="F8" t="b">
+        <v>1</v>
       </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>3</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1111</v>
       </c>
       <c r="B9" t="s">
         <v>1112</v>
       </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>1305</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>200</v>
       </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="b">
         <v>1</v>
       </c>
       <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>30</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1113</v>
       </c>
       <c r="B10" t="s">
         <v>1114</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D10">
         <v>500</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>2000</v>
       </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
+      <c r="F10" t="b">
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>45</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>1256</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1115</v>
       </c>
       <c r="B11" t="s">
         <v>1116</v>
       </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>1307</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>1800</v>
       </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="b">
         <v>1</v>
       </c>
       <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>180</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>1257</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1117</v>
       </c>
       <c r="B12" t="s">
         <v>1118</v>
       </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>1308</v>
       </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>50</v>
       </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12">
         <v>4</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>60</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>1258</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>206</v>
       </c>
       <c r="B13" t="s">
         <v>1119</v>
       </c>
-      <c r="C13">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>1309</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>30</v>
       </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>4</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>60</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1120</v>
       </c>
       <c r="B14" t="s">
         <v>1121</v>
       </c>
-      <c r="C14">
-        <v>0</v>
+      <c r="C14" t="s">
+        <v>1310</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>100</v>
       </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>10</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>1136</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1122</v>
       </c>
       <c r="B15" t="s">
         <v>1123</v>
       </c>
-      <c r="C15">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>1311</v>
       </c>
       <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>400</v>
       </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="b">
         <v>1</v>
       </c>
       <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <v>120</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>1260</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1124</v>
       </c>
       <c r="B16" t="s">
         <v>1102</v>
       </c>
-      <c r="C16">
-        <v>0</v>
+      <c r="C16" t="s">
+        <v>1300</v>
       </c>
       <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>300</v>
       </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>160</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>419</v>
       </c>
       <c r="B17" t="s">
         <v>1125</v>
       </c>
-      <c r="C17">
-        <v>0</v>
+      <c r="C17" t="s">
+        <v>1312</v>
       </c>
       <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>125</v>
       </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
-      <c r="G17">
+      <c r="G17" t="b">
         <v>1</v>
       </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>300</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1126</v>
       </c>
       <c r="B18" t="s">
         <v>1127</v>
       </c>
-      <c r="C18">
-        <v>0</v>
+      <c r="C18" t="s">
+        <v>1127</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>120</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>1261</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1128</v>
       </c>
       <c r="B19" t="s">
         <v>1128</v>
       </c>
-      <c r="C19">
-        <v>0</v>
+      <c r="C19" t="s">
+        <v>1128</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -30000,24 +30277,27 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
         <v>1262</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
       <c r="B20" t="s">
         <v>1129</v>
       </c>
-      <c r="C20">
-        <v>0</v>
+      <c r="C20" t="s">
+        <v>1129</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -30029,1830 +30309,2022 @@
         <v>0</v>
       </c>
       <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>60</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>1263</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1130</v>
       </c>
       <c r="B21" t="s">
         <v>1131</v>
       </c>
-      <c r="C21">
-        <v>0</v>
+      <c r="C21" t="s">
+        <v>1313</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>665</v>
       </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
-      <c r="G21">
+      <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <v>120</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1132</v>
       </c>
       <c r="B22" t="s">
         <v>1133</v>
       </c>
-      <c r="C22">
-        <v>0</v>
+      <c r="C22" t="s">
+        <v>1314</v>
       </c>
       <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>10</v>
       </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
-      <c r="G22">
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>5</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>60</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>1132</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1134</v>
       </c>
       <c r="B23" t="s">
         <v>1135</v>
       </c>
-      <c r="C23">
-        <v>0</v>
+      <c r="C23" t="s">
+        <v>1315</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
         <v>50</v>
       </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
-      <c r="G23">
+      <c r="G23" t="b">
         <v>1</v>
       </c>
       <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <v>60</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>1264</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1136</v>
       </c>
       <c r="B24" t="s">
         <v>1137</v>
       </c>
-      <c r="C24">
-        <v>0</v>
+      <c r="C24" t="s">
+        <v>1310</v>
       </c>
       <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
         <v>2</v>
       </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="b">
         <v>1</v>
       </c>
       <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
         <v>120</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>1136</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1138</v>
       </c>
       <c r="B25" t="s">
         <v>1139</v>
       </c>
-      <c r="C25">
-        <v>0</v>
+      <c r="C25" t="s">
+        <v>1316</v>
       </c>
       <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
         <v>2</v>
       </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
-      <c r="G25">
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25">
         <v>5</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>60</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1140</v>
       </c>
       <c r="B26" t="s">
         <v>1141</v>
       </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="C26" t="s">
+        <v>1317</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
       </c>
       <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>2</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>120</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1142</v>
       </c>
       <c r="B27" t="s">
         <v>1143</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D27">
         <v>5000</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>5</v>
       </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
-      <c r="G27">
+      <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>120</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>1265</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>511</v>
       </c>
       <c r="B28" t="s">
         <v>1144</v>
       </c>
-      <c r="C28">
-        <v>0</v>
+      <c r="C28" t="s">
+        <v>1319</v>
       </c>
       <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
         <v>2</v>
       </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
-      <c r="G28">
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <v>5</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>60</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1145</v>
       </c>
       <c r="B29" t="s">
         <v>1146</v>
       </c>
-      <c r="C29">
-        <v>0</v>
+      <c r="C29" t="s">
+        <v>1320</v>
       </c>
       <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
         <v>70</v>
       </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
       <c r="F29" t="b">
         <v>1</v>
       </c>
-      <c r="G29">
+      <c r="G29" t="b">
         <v>1</v>
       </c>
       <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <v>10</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1147</v>
       </c>
       <c r="B30" t="s">
         <v>1148</v>
       </c>
-      <c r="C30">
-        <v>0</v>
+      <c r="C30" t="s">
+        <v>1321</v>
       </c>
       <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>200</v>
       </c>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
       <c r="F30" t="b">
         <v>1</v>
       </c>
-      <c r="G30">
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30">
         <v>2</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>120</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>1266</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1149</v>
       </c>
       <c r="B31" t="s">
         <v>1150</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D31">
         <v>10000</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>150</v>
       </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
+      <c r="F31" t="b">
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
         <v>20</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>1267</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1151</v>
       </c>
       <c r="B32" t="s">
         <v>1152</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D32">
         <v>100000</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>150</v>
       </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
       <c r="F32" t="b">
         <v>1</v>
       </c>
-      <c r="G32">
+      <c r="G32" t="b">
         <v>1</v>
       </c>
       <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <v>120</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>1268</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1153</v>
       </c>
       <c r="B33" t="s">
         <v>1154</v>
       </c>
-      <c r="C33">
-        <v>0</v>
+      <c r="C33" t="s">
+        <v>1324</v>
       </c>
       <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
         <v>70</v>
       </c>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
       <c r="F33" t="b">
         <v>1</v>
       </c>
-      <c r="G33">
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33">
         <v>2</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>30</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1155</v>
       </c>
       <c r="B34" t="s">
         <v>1156</v>
       </c>
-      <c r="C34">
-        <v>0</v>
+      <c r="C34" t="s">
+        <v>1325</v>
       </c>
       <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
         <v>2</v>
       </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
       <c r="F34" t="b">
         <v>1</v>
       </c>
-      <c r="G34">
+      <c r="G34" t="b">
         <v>1</v>
       </c>
       <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
         <v>120</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>1269</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1157</v>
       </c>
       <c r="B35" t="s">
         <v>1158</v>
       </c>
-      <c r="C35">
-        <v>0</v>
+      <c r="C35" t="s">
+        <v>1326</v>
       </c>
       <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
         <v>50</v>
       </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
       <c r="F35" t="b">
         <v>1</v>
       </c>
-      <c r="G35">
+      <c r="G35" t="b">
         <v>1</v>
       </c>
       <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
         <v>90</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>1270</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1159</v>
       </c>
       <c r="B36" t="s">
         <v>1160</v>
       </c>
-      <c r="C36">
-        <v>0</v>
+      <c r="C36" t="s">
+        <v>1327</v>
       </c>
       <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
         <v>250</v>
       </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
       <c r="F36" t="b">
         <v>1</v>
       </c>
-      <c r="G36">
+      <c r="G36" t="b">
         <v>1</v>
       </c>
       <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
         <v>120</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>1159</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1161</v>
       </c>
       <c r="B37" t="s">
         <v>1162</v>
       </c>
-      <c r="C37">
-        <v>0</v>
+      <c r="C37" t="s">
+        <v>1328</v>
       </c>
       <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>200</v>
       </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
       <c r="F37" t="b">
         <v>1</v>
       </c>
-      <c r="G37">
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37">
         <v>2</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>120</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>1161</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1163</v>
       </c>
       <c r="B38" t="s">
         <v>1164</v>
       </c>
-      <c r="C38">
-        <v>0</v>
+      <c r="C38" t="s">
+        <v>1329</v>
       </c>
       <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
         <v>100</v>
       </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
       <c r="F38" t="b">
         <v>1</v>
       </c>
-      <c r="G38">
+      <c r="G38" t="b">
         <v>1</v>
       </c>
       <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
         <v>30</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>1271</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1165</v>
       </c>
       <c r="B39" t="s">
         <v>1166</v>
       </c>
-      <c r="C39">
-        <v>0</v>
+      <c r="C39" t="s">
+        <v>1330</v>
       </c>
       <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
         <v>30</v>
       </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
       <c r="F39" t="b">
         <v>1</v>
       </c>
-      <c r="G39">
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39">
         <v>5</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>120</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1167</v>
       </c>
       <c r="B40" t="s">
         <v>1168</v>
       </c>
-      <c r="C40">
-        <v>0</v>
+      <c r="C40" t="s">
+        <v>1331</v>
       </c>
       <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
         <v>150</v>
       </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
       <c r="F40" t="b">
         <v>1</v>
       </c>
-      <c r="G40">
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40">
         <v>2</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>60</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1169</v>
       </c>
       <c r="B41" t="s">
         <v>1170</v>
       </c>
-      <c r="C41">
-        <v>0</v>
+      <c r="C41" t="s">
+        <v>1332</v>
       </c>
       <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
         <v>50</v>
       </c>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
       <c r="F41" t="b">
         <v>1</v>
       </c>
-      <c r="G41">
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41">
         <v>2</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>60</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1171</v>
       </c>
       <c r="B42" t="s">
         <v>1172</v>
       </c>
-      <c r="C42">
-        <v>0</v>
+      <c r="C42" t="s">
+        <v>1333</v>
       </c>
       <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
         <v>150</v>
       </c>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
       <c r="F42" t="b">
         <v>1</v>
       </c>
-      <c r="G42">
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42">
         <v>3</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>120</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1173</v>
       </c>
       <c r="B43" t="s">
         <v>1174</v>
       </c>
-      <c r="C43">
-        <v>0</v>
+      <c r="C43" t="s">
+        <v>1334</v>
       </c>
       <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>6</v>
       </c>
-      <c r="E43" t="b">
-        <v>1</v>
-      </c>
       <c r="F43" t="b">
         <v>1</v>
       </c>
-      <c r="G43">
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43">
         <v>5</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>60</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>1276</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1175</v>
       </c>
       <c r="B44" t="s">
         <v>1176</v>
       </c>
-      <c r="C44">
-        <v>0</v>
+      <c r="C44" t="s">
+        <v>1335</v>
       </c>
       <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
         <v>150</v>
       </c>
-      <c r="E44" t="b">
-        <v>1</v>
-      </c>
       <c r="F44" t="b">
         <v>1</v>
       </c>
-      <c r="G44">
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44">
         <v>5</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>120</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1177</v>
       </c>
       <c r="B45" t="s">
         <v>1178</v>
       </c>
-      <c r="C45">
-        <v>0</v>
+      <c r="C45" t="s">
+        <v>1336</v>
       </c>
       <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
         <v>850</v>
       </c>
-      <c r="E45" t="b">
-        <v>1</v>
-      </c>
       <c r="F45" t="b">
         <v>1</v>
       </c>
-      <c r="G45">
+      <c r="G45" t="b">
         <v>1</v>
       </c>
       <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
         <v>60</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1179</v>
       </c>
       <c r="B46" t="s">
         <v>1180</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D46">
         <v>250</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>300</v>
       </c>
-      <c r="E46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="F46" t="b">
+        <v>1</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
         <v>45</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>1267</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1181</v>
       </c>
       <c r="B47" t="s">
         <v>1182</v>
       </c>
-      <c r="C47">
-        <v>0</v>
+      <c r="C47" t="s">
+        <v>1337</v>
       </c>
       <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
         <v>2</v>
       </c>
-      <c r="E47" t="b">
-        <v>1</v>
-      </c>
       <c r="F47" t="b">
         <v>1</v>
       </c>
-      <c r="G47">
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47">
         <v>5</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>60</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1183</v>
       </c>
       <c r="B48" t="s">
         <v>1184</v>
       </c>
-      <c r="C48">
-        <v>0</v>
+      <c r="C48" t="s">
+        <v>1338</v>
       </c>
       <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
         <v>800</v>
       </c>
-      <c r="E48" t="b">
-        <v>1</v>
-      </c>
       <c r="F48" t="b">
         <v>1</v>
       </c>
-      <c r="G48">
+      <c r="G48" t="b">
         <v>1</v>
       </c>
       <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
         <v>120</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1185</v>
       </c>
       <c r="B49" t="s">
         <v>1186</v>
       </c>
-      <c r="C49">
-        <v>0</v>
+      <c r="C49" t="s">
+        <v>1339</v>
       </c>
       <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
         <v>100</v>
       </c>
-      <c r="E49" t="b">
-        <v>1</v>
-      </c>
       <c r="F49" t="b">
         <v>1</v>
       </c>
-      <c r="G49">
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49">
         <v>2</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>120</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>1279</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1187</v>
       </c>
       <c r="B50" t="s">
         <v>1188</v>
       </c>
-      <c r="C50">
-        <v>0</v>
+      <c r="C50" t="s">
+        <v>1340</v>
       </c>
       <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
         <v>400</v>
       </c>
-      <c r="E50" t="b">
-        <v>1</v>
-      </c>
       <c r="F50" t="b">
         <v>1</v>
       </c>
-      <c r="G50">
+      <c r="G50" t="b">
         <v>1</v>
       </c>
       <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
         <v>120</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1189</v>
       </c>
       <c r="B51" t="s">
         <v>1190</v>
       </c>
-      <c r="C51">
-        <v>0</v>
+      <c r="C51" t="s">
+        <v>1341</v>
       </c>
       <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
         <v>100</v>
       </c>
-      <c r="E51" t="b">
-        <v>1</v>
-      </c>
       <c r="F51" t="b">
         <v>1</v>
       </c>
-      <c r="G51">
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51">
         <v>2</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>90</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>1189</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1191</v>
       </c>
       <c r="B52" t="s">
         <v>1192</v>
       </c>
-      <c r="C52">
-        <v>0</v>
+      <c r="C52" t="s">
+        <v>1342</v>
       </c>
       <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
         <v>200</v>
       </c>
-      <c r="E52" t="b">
-        <v>1</v>
-      </c>
       <c r="F52" t="b">
         <v>1</v>
       </c>
-      <c r="G52">
+      <c r="G52" t="b">
         <v>1</v>
       </c>
       <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1193</v>
       </c>
       <c r="B53" t="s">
         <v>1194</v>
       </c>
-      <c r="C53">
-        <v>0</v>
+      <c r="C53" t="s">
+        <v>1343</v>
       </c>
       <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
         <v>2</v>
       </c>
-      <c r="E53" t="b">
-        <v>1</v>
-      </c>
       <c r="F53" t="b">
         <v>1</v>
       </c>
-      <c r="G53">
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53">
         <v>5</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>60</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>1281</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1195</v>
       </c>
       <c r="B54" t="s">
         <v>1196</v>
       </c>
-      <c r="C54">
-        <v>0</v>
+      <c r="C54" t="s">
+        <v>1344</v>
       </c>
       <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
         <v>325</v>
       </c>
-      <c r="E54" t="b">
-        <v>1</v>
-      </c>
       <c r="F54" t="b">
         <v>1</v>
       </c>
-      <c r="G54">
+      <c r="G54" t="b">
         <v>1</v>
       </c>
       <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
         <v>120</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>1282</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1122</v>
       </c>
       <c r="B55" t="s">
         <v>1197</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D55">
         <v>10000</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
       <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>25</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>120</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>1283</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1173</v>
       </c>
       <c r="B56" t="s">
         <v>1198</v>
       </c>
-      <c r="C56">
-        <v>0</v>
+      <c r="C56" t="s">
+        <v>1346</v>
       </c>
       <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
         <v>15</v>
       </c>
-      <c r="E56" t="b">
-        <v>1</v>
-      </c>
       <c r="F56" t="b">
         <v>1</v>
       </c>
-      <c r="G56">
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56">
         <v>5</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>60</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>1276</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1199</v>
       </c>
       <c r="B57" t="s">
         <v>1200</v>
       </c>
-      <c r="C57">
-        <v>0</v>
+      <c r="C57" t="s">
+        <v>1347</v>
       </c>
       <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
         <v>100</v>
       </c>
-      <c r="E57" t="b">
-        <v>1</v>
-      </c>
       <c r="F57" t="b">
         <v>1</v>
       </c>
-      <c r="G57">
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57">
         <v>2</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>60</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>1199</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1201</v>
       </c>
       <c r="B58" t="s">
         <v>1202</v>
       </c>
-      <c r="C58">
-        <v>0</v>
+      <c r="C58" t="s">
+        <v>1348</v>
       </c>
       <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
         <v>2</v>
       </c>
-      <c r="E58" t="b">
-        <v>1</v>
-      </c>
       <c r="F58" t="b">
         <v>1</v>
       </c>
-      <c r="G58">
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58">
         <v>3</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>120</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>1284</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1203</v>
       </c>
       <c r="B59" t="s">
         <v>1204</v>
       </c>
-      <c r="C59">
-        <v>0</v>
+      <c r="C59" t="s">
+        <v>1349</v>
       </c>
       <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
         <v>75</v>
       </c>
-      <c r="E59" t="b">
-        <v>1</v>
-      </c>
       <c r="F59" t="b">
         <v>1</v>
       </c>
-      <c r="G59">
+      <c r="G59" t="b">
         <v>1</v>
       </c>
       <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
         <v>60</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>1203</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1205</v>
       </c>
       <c r="B60" t="s">
         <v>1206</v>
       </c>
-      <c r="C60">
-        <v>0</v>
+      <c r="C60" t="s">
+        <v>1350</v>
       </c>
       <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
         <v>400</v>
       </c>
-      <c r="E60" t="b">
-        <v>1</v>
-      </c>
       <c r="F60" t="b">
         <v>1</v>
       </c>
-      <c r="G60">
+      <c r="G60" t="b">
         <v>1</v>
       </c>
       <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
         <v>120</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>1285</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1207</v>
       </c>
       <c r="B61" t="s">
         <v>1208</v>
       </c>
-      <c r="C61">
-        <v>0</v>
+      <c r="C61" t="s">
+        <v>1351</v>
       </c>
       <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
         <v>210</v>
       </c>
-      <c r="E61" t="b">
-        <v>1</v>
-      </c>
       <c r="F61" t="b">
         <v>1</v>
       </c>
-      <c r="G61">
+      <c r="G61" t="b">
         <v>1</v>
       </c>
       <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
         <v>180</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1209</v>
       </c>
       <c r="B62" t="s">
         <v>1210</v>
       </c>
-      <c r="C62">
-        <v>0</v>
+      <c r="C62" t="s">
+        <v>1352</v>
       </c>
       <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
         <v>40</v>
       </c>
-      <c r="E62" t="b">
-        <v>1</v>
-      </c>
       <c r="F62" t="b">
         <v>1</v>
       </c>
-      <c r="G62">
+      <c r="G62" t="b">
         <v>1</v>
       </c>
       <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
         <v>10</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>1209</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>423</v>
       </c>
       <c r="B63" t="s">
         <v>1211</v>
       </c>
-      <c r="C63">
-        <v>0</v>
+      <c r="C63" t="s">
+        <v>1353</v>
       </c>
       <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
         <v>290</v>
       </c>
-      <c r="E63" t="b">
-        <v>1</v>
-      </c>
       <c r="F63" t="b">
         <v>1</v>
       </c>
-      <c r="G63">
+      <c r="G63" t="b">
         <v>1</v>
       </c>
       <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
         <v>120</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1212</v>
       </c>
       <c r="B64" t="s">
         <v>1213</v>
       </c>
-      <c r="C64">
+      <c r="C64" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D64">
         <v>250</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>50</v>
       </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
+      <c r="F64" t="b">
+        <v>1</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
         <v>20</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>1287</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1214</v>
       </c>
       <c r="B65" t="s">
         <v>1215</v>
       </c>
-      <c r="C65">
+      <c r="C65" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D65">
         <v>5000</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>10</v>
       </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
       <c r="F65" t="b">
         <v>1</v>
       </c>
-      <c r="G65">
+      <c r="G65" t="b">
         <v>1</v>
       </c>
       <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
         <v>120</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>1288</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1216</v>
       </c>
       <c r="B66" t="s">
         <v>1217</v>
       </c>
-      <c r="C66">
+      <c r="C66" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D66">
         <v>185</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>600</v>
       </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
       <c r="F66" t="b">
         <v>1</v>
       </c>
-      <c r="G66">
+      <c r="G66" t="b">
         <v>1</v>
       </c>
       <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
         <v>120</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>1258</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1218</v>
       </c>
       <c r="B67" t="s">
         <v>1219</v>
       </c>
-      <c r="C67">
-        <v>0</v>
+      <c r="C67" t="s">
+        <v>1357</v>
       </c>
       <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
         <v>15</v>
       </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
       <c r="F67" t="b">
         <v>1</v>
       </c>
-      <c r="G67">
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67">
         <v>5</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>60</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1220</v>
       </c>
       <c r="B68" t="s">
         <v>1221</v>
       </c>
-      <c r="C68">
-        <v>0</v>
+      <c r="C68" t="s">
+        <v>1358</v>
       </c>
       <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
         <v>275</v>
       </c>
-      <c r="E68" t="b">
-        <v>1</v>
-      </c>
       <c r="F68" t="b">
         <v>1</v>
       </c>
-      <c r="G68">
+      <c r="G68" t="b">
         <v>1</v>
       </c>
       <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
         <v>300</v>
       </c>
-      <c r="I68" t="s">
+      <c r="J68" t="s">
         <v>1289</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1222</v>
       </c>
       <c r="B69" t="s">
         <v>1223</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D69">
         <v>2500</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>35</v>
       </c>
-      <c r="E69" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
+      <c r="F69" t="b">
+        <v>1</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
         <v>20</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" t="s">
         <v>1287</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1224</v>
       </c>
       <c r="B70" t="s">
         <v>1225</v>
       </c>
-      <c r="C70">
-        <v>0</v>
+      <c r="C70" t="s">
+        <v>1359</v>
       </c>
       <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
         <v>3275</v>
       </c>
-      <c r="E70" t="b">
-        <v>1</v>
-      </c>
       <c r="F70" t="b">
         <v>1</v>
       </c>
-      <c r="G70">
+      <c r="G70" t="b">
         <v>1</v>
       </c>
       <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
         <v>60</v>
       </c>
-      <c r="I70" t="s">
+      <c r="J70" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1226</v>
       </c>
       <c r="B71" t="s">
         <v>1227</v>
       </c>
-      <c r="C71">
+      <c r="C71" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D71">
         <v>1000</v>
       </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71" t="b">
-        <v>1</v>
+      <c r="E71">
+        <v>0</v>
       </c>
       <c r="F71" t="b">
         <v>1</v>
       </c>
-      <c r="G71">
+      <c r="G71" t="b">
         <v>1</v>
       </c>
       <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
         <v>120</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1228</v>
       </c>
       <c r="B72" t="s">
         <v>1229</v>
       </c>
-      <c r="C72">
+      <c r="C72" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D72">
         <v>500</v>
       </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72" t="b">
-        <v>1</v>
+      <c r="E72">
+        <v>0</v>
       </c>
       <c r="F72" t="b">
         <v>1</v>
       </c>
-      <c r="G72">
+      <c r="G72" t="b">
         <v>1</v>
       </c>
       <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1230</v>
       </c>
       <c r="B73" t="s">
         <v>1231</v>
       </c>
-      <c r="C73">
-        <v>0</v>
+      <c r="C73" t="s">
+        <v>1362</v>
       </c>
       <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
         <v>50</v>
       </c>
-      <c r="E73" t="b">
-        <v>1</v>
-      </c>
       <c r="F73" t="b">
         <v>1</v>
       </c>
-      <c r="G73">
+      <c r="G73" t="b">
         <v>1</v>
       </c>
       <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
         <v>120</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1232</v>
       </c>
       <c r="B74" t="s">
         <v>1233</v>
       </c>
-      <c r="C74">
+      <c r="C74" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D74">
         <v>20000</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>5</v>
       </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
       <c r="F74" t="b">
         <v>1</v>
       </c>
-      <c r="G74">
+      <c r="G74" t="b">
         <v>1</v>
       </c>
       <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
         <v>120</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>1293</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1234</v>
       </c>
       <c r="B75" t="s">
         <v>1235</v>
       </c>
-      <c r="C75">
+      <c r="C75" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D75">
         <v>5000</v>
       </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="E75" t="b">
+      <c r="E75">
         <v>1</v>
       </c>
       <c r="F75" t="b">
         <v>1</v>
       </c>
-      <c r="G75">
+      <c r="G75" t="b">
         <v>1</v>
       </c>
       <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
         <v>120</v>
       </c>
-      <c r="I75" t="s">
+      <c r="J75" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1236</v>
       </c>
       <c r="B76" t="s">
         <v>1237</v>
       </c>
-      <c r="C76">
-        <v>0</v>
+      <c r="C76" t="s">
+        <v>1365</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
-      <c r="E76" t="b">
-        <v>1</v>
+      <c r="E76">
+        <v>0</v>
       </c>
       <c r="F76" t="b">
         <v>1</v>
       </c>
-      <c r="G76">
+      <c r="G76" t="b">
         <v>1</v>
       </c>
       <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1238</v>
       </c>
       <c r="B77" t="s">
         <v>1239</v>
       </c>
-      <c r="C77">
-        <v>0</v>
+      <c r="C77" t="s">
+        <v>1239</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
-      <c r="E77" t="b">
-        <v>1</v>
+      <c r="E77">
+        <v>0</v>
       </c>
       <c r="F77" t="b">
         <v>1</v>
       </c>
-      <c r="G77">
+      <c r="G77" t="b">
         <v>1</v>
       </c>
       <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
         <v>120</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1240</v>
       </c>
       <c r="B78" t="s">
         <v>1241</v>
       </c>
-      <c r="C78">
+      <c r="C78" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D78">
         <v>2500</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>5</v>
       </c>
-      <c r="E78" t="b">
-        <v>1</v>
-      </c>
       <c r="F78" t="b">
         <v>1</v>
       </c>
-      <c r="G78">
+      <c r="G78" t="b">
         <v>1</v>
       </c>
       <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
         <v>120</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>1294</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1242</v>
       </c>
       <c r="B79" t="s">
         <v>1243</v>
       </c>
-      <c r="C79">
-        <v>0</v>
+      <c r="C79" t="s">
+        <v>1367</v>
       </c>
       <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
         <v>400</v>
       </c>
-      <c r="E79" t="b">
-        <v>1</v>
-      </c>
       <c r="F79" t="b">
         <v>1</v>
       </c>
-      <c r="G79">
+      <c r="G79" t="b">
         <v>1</v>
       </c>
       <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
         <v>120</v>
       </c>
-      <c r="I79" t="s">
+      <c r="J79" t="s">
         <v>1295</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1244</v>
       </c>
       <c r="B80" t="s">
         <v>1245</v>
       </c>
-      <c r="C80">
-        <v>0</v>
+      <c r="C80" t="s">
+        <v>1368</v>
       </c>
       <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
         <v>50</v>
       </c>
-      <c r="E80" t="b">
-        <v>1</v>
-      </c>
       <c r="F80" t="b">
         <v>1</v>
       </c>
-      <c r="G80">
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+      <c r="H80">
         <v>2</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <v>60</v>
       </c>
-      <c r="I80" t="s">
+      <c r="J80" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1246</v>
       </c>
       <c r="B81" t="s">
         <v>1247</v>
       </c>
-      <c r="C81">
+      <c r="C81" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D81">
         <v>2000</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>5</v>
       </c>
-      <c r="E81" t="b">
-        <v>1</v>
-      </c>
       <c r="F81" t="b">
         <v>1</v>
       </c>
-      <c r="G81">
+      <c r="G81" t="b">
         <v>1</v>
       </c>
       <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
         <v>120</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>1296</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1248</v>
       </c>
       <c r="B82" t="s">
         <v>1249</v>
       </c>
-      <c r="C82">
+      <c r="C82" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D82">
         <v>20</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>30</v>
       </c>
-      <c r="E82" t="b">
-        <v>1</v>
-      </c>
       <c r="F82" t="b">
         <v>1</v>
       </c>
-      <c r="G82">
+      <c r="G82" t="b">
+        <v>1</v>
+      </c>
+      <c r="H82">
         <v>3</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>30</v>
       </c>
-      <c r="I82" t="s">
+      <c r="J82" t="s">
         <v>1297</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1250</v>
       </c>
       <c r="B83" t="s">
         <v>1251</v>
       </c>
-      <c r="C83">
-        <v>0</v>
+      <c r="C83" t="s">
+        <v>1371</v>
       </c>
       <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
         <v>800</v>
       </c>
-      <c r="E83" t="b">
-        <v>1</v>
-      </c>
       <c r="F83" t="b">
         <v>1</v>
       </c>
-      <c r="G83">
+      <c r="G83" t="b">
         <v>1</v>
       </c>
       <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
         <v>600</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>406</v>
       </c>
     </row>

</xml_diff>